<commit_message>
Fix bright+ button on 38-key remote.
</commit_message>
<xml_diff>
--- a/IR_Remote_Codes.xlsx
+++ b/IR_Remote_Codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\WLED\WLED-Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DCEDF3-4B50-41B5-9622-EFC476307301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ACDCBF-81C4-4C10-A96C-F024A8143889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8505" yWindow="885" windowWidth="18105" windowHeight="13485" tabRatio="788" firstSheet="4" activeTab="10" xr2:uid="{A5B47F4F-92F9-44F8-AB67-245490107EC0}"/>
+    <workbookView xWindow="8505" yWindow="885" windowWidth="18105" windowHeight="13485" tabRatio="788" firstSheet="4" activeTab="9" xr2:uid="{A5B47F4F-92F9-44F8-AB67-245490107EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="6-key" sheetId="8" r:id="rId1"/>
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D17498-88C9-4394-9FEC-76D4CB2FA9BC}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2095,7 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="D31" t="s">
         <v>150</v>
@@ -2258,7 +2258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B38EC3C-D835-4B08-84A7-0D994D2DDC9F}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>

</xml_diff>

<commit_message>
Add IR support for Athom controller
</commit_message>
<xml_diff>
--- a/IR_Remote_Codes.xlsx
+++ b/IR_Remote_Codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\WLED\WLED-Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ACDCBF-81C4-4C10-A96C-F024A8143889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BD5CCA-4F57-45AA-96C8-95001EEDE46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8505" yWindow="885" windowWidth="18105" windowHeight="13485" tabRatio="788" firstSheet="4" activeTab="9" xr2:uid="{A5B47F4F-92F9-44F8-AB67-245490107EC0}"/>
+    <workbookView xWindow="75" yWindow="600" windowWidth="15045" windowHeight="14025" tabRatio="788" firstSheet="5" activeTab="8" xr2:uid="{A5B47F4F-92F9-44F8-AB67-245490107EC0}"/>
   </bookViews>
   <sheets>
     <sheet name="6-key" sheetId="8" r:id="rId1"/>
@@ -21,11 +21,12 @@
     <sheet name="24-key-grey" sheetId="13" r:id="rId6"/>
     <sheet name="24-key-v2" sheetId="10" r:id="rId7"/>
     <sheet name="24-key-v3" sheetId="3" r:id="rId8"/>
-    <sheet name="32-key" sheetId="1" r:id="rId9"/>
-    <sheet name="38-key" sheetId="12" r:id="rId10"/>
-    <sheet name="40-key-blue" sheetId="4" r:id="rId11"/>
-    <sheet name="40-key-black" sheetId="2" r:id="rId12"/>
-    <sheet name="44-key" sheetId="5" r:id="rId13"/>
+    <sheet name="24-key-Athom" sheetId="14" r:id="rId9"/>
+    <sheet name="32-key" sheetId="1" r:id="rId10"/>
+    <sheet name="38-key" sheetId="12" r:id="rId11"/>
+    <sheet name="40-key-blue" sheetId="4" r:id="rId12"/>
+    <sheet name="40-key-black" sheetId="2" r:id="rId13"/>
+    <sheet name="44-key" sheetId="5" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="342">
   <si>
     <t>0xF700FF</t>
   </si>
@@ -846,9 +847,6 @@
     <t>W=~16</t>
   </si>
   <si>
-    <t>W=-16</t>
-  </si>
-  <si>
     <t>R=0&amp;G=0&amp;B=0&amp;W=255</t>
   </si>
   <si>
@@ -1054,6 +1052,27 @@
   </si>
   <si>
     <t>Meteor Smooth-Redwhi</t>
+  </si>
+  <si>
+    <t>Plumb</t>
+  </si>
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>FX=0</t>
+  </si>
+  <si>
+    <t>Set effect to solid</t>
+  </si>
+  <si>
+    <t>W=~-16</t>
+  </si>
+  <si>
+    <t>Preset-</t>
+  </si>
+  <si>
+    <t>Preset+</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1514,7 @@
         <v>242</v>
       </c>
       <c r="E3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1518,7 +1537,7 @@
         <v>243</v>
       </c>
       <c r="E4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1564,7 +1583,7 @@
         <v>133</v>
       </c>
       <c r="J6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1581,7 +1600,7 @@
         <v>246</v>
       </c>
       <c r="E7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J7" t="s">
         <v>9</v>
@@ -1593,11 +1612,608 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E99131-E2A9-44CA-9411-B82003F38B39}">
+  <dimension ref="A1:J33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s">
+        <v>191</v>
+      </c>
+      <c r="J7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" t="s">
+        <v>269</v>
+      </c>
+      <c r="G22" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" t="s">
+        <v>197</v>
+      </c>
+      <c r="I22" t="s">
+        <v>198</v>
+      </c>
+      <c r="J22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>293</v>
+      </c>
+      <c r="J26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" t="s">
+        <v>292</v>
+      </c>
+      <c r="J27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D30" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" t="s">
+        <v>278</v>
+      </c>
+      <c r="J30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" t="s">
+        <v>296</v>
+      </c>
+      <c r="J31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" t="s">
+        <v>295</v>
+      </c>
+      <c r="J32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" t="s">
+        <v>294</v>
+      </c>
+      <c r="J33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3D17498-88C9-4394-9FEC-76D4CB2FA9BC}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J1" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,16 +2389,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D11" t="s">
         <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -1835,16 +2451,16 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D15" t="s">
         <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1897,16 +2513,16 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D19" t="s">
         <v>62</v>
       </c>
       <c r="E19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="J19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1923,7 +2539,7 @@
         <v>134</v>
       </c>
       <c r="E20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G20" t="s">
         <v>91</v>
@@ -1935,7 +2551,7 @@
         <v>198</v>
       </c>
       <c r="J20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1974,16 +2590,16 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D23" t="s">
         <v>67</v>
       </c>
       <c r="E23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1994,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D24" t="s">
         <v>102</v>
@@ -2008,7 +2624,7 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D25" t="s">
         <v>69</v>
@@ -2022,7 +2638,7 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D26" t="s">
         <v>77</v>
@@ -2036,7 +2652,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D27" t="s">
         <v>73</v>
@@ -2050,13 +2666,13 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D28" t="s">
         <v>49</v>
       </c>
       <c r="J28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2067,7 +2683,7 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D29" t="s">
         <v>68</v>
@@ -2081,7 +2697,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D30" t="s">
         <v>75</v>
@@ -2095,7 +2711,7 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D31" t="s">
         <v>150</v>
@@ -2109,16 +2725,16 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D32" t="s">
         <v>105</v>
       </c>
       <c r="E32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -2129,16 +2745,16 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D33" t="s">
         <v>64</v>
       </c>
       <c r="E33" t="s">
+        <v>326</v>
+      </c>
+      <c r="J33" t="s">
         <v>327</v>
-      </c>
-      <c r="J33" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2149,7 +2765,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D34" t="s">
         <v>95</v>
@@ -2163,7 +2779,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D35" t="s">
         <v>104</v>
@@ -2177,16 +2793,16 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D36" t="s">
         <v>154</v>
       </c>
       <c r="E36" t="s">
+        <v>312</v>
+      </c>
+      <c r="J36" t="s">
         <v>313</v>
-      </c>
-      <c r="J36" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -2197,16 +2813,16 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D37" t="s">
         <v>58</v>
       </c>
       <c r="E37" t="s">
+        <v>314</v>
+      </c>
+      <c r="J37" t="s">
         <v>315</v>
-      </c>
-      <c r="J37" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2217,16 +2833,16 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D38" t="s">
         <v>90</v>
       </c>
       <c r="E38" t="s">
+        <v>316</v>
+      </c>
+      <c r="J38" t="s">
         <v>317</v>
-      </c>
-      <c r="J38" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2237,16 +2853,16 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D39" t="s">
         <v>158</v>
       </c>
       <c r="E39" t="s">
+        <v>318</v>
+      </c>
+      <c r="J39" t="s">
         <v>319</v>
-      </c>
-      <c r="J39" t="s">
-        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -2254,13 +2870,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B38EC3C-D835-4B08-84A7-0D994D2DDC9F}">
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2523,7 +3139,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D17" t="s">
         <v>83</v>
@@ -2605,7 +3221,7 @@
         <v>134</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" t="s">
         <v>91</v>
@@ -2617,7 +3233,7 @@
         <v>198</v>
       </c>
       <c r="J22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2699,7 +3315,7 @@
         <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>266</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2716,7 +3332,7 @@
         <v>77</v>
       </c>
       <c r="E28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2818,7 +3434,7 @@
         <v>105</v>
       </c>
       <c r="E34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J34" t="s">
         <v>140</v>
@@ -2838,7 +3454,7 @@
         <v>64</v>
       </c>
       <c r="E35" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J35" t="s">
         <v>142</v>
@@ -2858,7 +3474,7 @@
         <v>95</v>
       </c>
       <c r="E36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J36" t="s">
         <v>146</v>
@@ -2892,7 +3508,7 @@
         <v>154</v>
       </c>
       <c r="E38" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J38" t="s">
         <v>148</v>
@@ -2932,7 +3548,7 @@
         <v>90</v>
       </c>
       <c r="J40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2954,13 +3570,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADC6FE3-3EF7-4710-A0B8-E74DED38FC1D}">
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3282,7 +3898,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D21" t="s">
         <v>62</v>
@@ -3302,7 +3918,7 @@
         <v>134</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" t="s">
         <v>91</v>
@@ -3314,7 +3930,7 @@
         <v>198</v>
       </c>
       <c r="J22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3353,7 +3969,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
@@ -3373,7 +3989,7 @@
         <v>102</v>
       </c>
       <c r="E26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J26" t="s">
         <v>140</v>
@@ -3393,7 +4009,7 @@
         <v>69</v>
       </c>
       <c r="E27" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J27" t="s">
         <v>142</v>
@@ -3447,7 +4063,7 @@
         <v>49</v>
       </c>
       <c r="E30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J30" t="s">
         <v>146</v>
@@ -3467,7 +4083,7 @@
         <v>68</v>
       </c>
       <c r="E31" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J31" t="s">
         <v>148</v>
@@ -3487,7 +4103,7 @@
         <v>75</v>
       </c>
       <c r="J32" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -3512,13 +4128,13 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D34" t="s">
         <v>105</v>
       </c>
       <c r="J34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3529,13 +4145,13 @@
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D35" t="s">
         <v>64</v>
       </c>
       <c r="J35" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3580,13 +4196,13 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D38" t="s">
         <v>154</v>
       </c>
       <c r="J38" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3597,13 +4213,13 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D39" t="s">
         <v>58</v>
       </c>
       <c r="J39" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -3646,13 +4262,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{302AA6DC-95EB-465C-93D3-5EBADFE02E83}">
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E26:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,7 +4533,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D17" t="s">
         <v>83</v>
@@ -3931,7 +4547,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D18" t="s">
         <v>99</v>
@@ -3973,7 +4589,7 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D21" t="s">
         <v>62</v>
@@ -3993,7 +4609,7 @@
         <v>134</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" t="s">
         <v>91</v>
@@ -4005,7 +4621,7 @@
         <v>198</v>
       </c>
       <c r="J22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -4044,7 +4660,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
@@ -4206,10 +4822,10 @@
         <v>105</v>
       </c>
       <c r="E34" t="s">
+        <v>312</v>
+      </c>
+      <c r="J34" t="s">
         <v>313</v>
-      </c>
-      <c r="J34" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -4226,10 +4842,10 @@
         <v>64</v>
       </c>
       <c r="E35" t="s">
+        <v>314</v>
+      </c>
+      <c r="J35" t="s">
         <v>315</v>
-      </c>
-      <c r="J35" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -4246,10 +4862,10 @@
         <v>95</v>
       </c>
       <c r="E36" t="s">
+        <v>316</v>
+      </c>
+      <c r="J36" t="s">
         <v>317</v>
-      </c>
-      <c r="J36" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -4280,10 +4896,10 @@
         <v>154</v>
       </c>
       <c r="E38" t="s">
+        <v>318</v>
+      </c>
+      <c r="J38" t="s">
         <v>319</v>
-      </c>
-      <c r="J38" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -4300,10 +4916,10 @@
         <v>58</v>
       </c>
       <c r="E39" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J39" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -4320,10 +4936,10 @@
         <v>90</v>
       </c>
       <c r="E40" t="s">
+        <v>326</v>
+      </c>
+      <c r="J40" t="s">
         <v>327</v>
-      </c>
-      <c r="J40" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -4360,7 +4976,7 @@
         <v>86</v>
       </c>
       <c r="E42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J42" t="s">
         <v>140</v>
@@ -4380,7 +4996,7 @@
         <v>115</v>
       </c>
       <c r="E43" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J43" t="s">
         <v>146</v>
@@ -4400,7 +5016,7 @@
         <v>55</v>
       </c>
       <c r="E44" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J44" t="s">
         <v>142</v>
@@ -4420,7 +5036,7 @@
         <v>211</v>
       </c>
       <c r="E45" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J45" t="s">
         <v>148</v>
@@ -4493,7 +5109,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D3" t="s">
         <v>123</v>
@@ -4501,7 +5117,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D4" t="s">
         <v>81</v>
@@ -4509,7 +5125,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D5" t="s">
         <v>239</v>
@@ -4551,7 +5167,7 @@
         <v>66</v>
       </c>
       <c r="E8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J8" t="s">
         <v>34</v>
@@ -4565,7 +5181,7 @@
         <v>99</v>
       </c>
       <c r="E9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
@@ -4688,7 +5304,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D5" t="s">
         <v>123</v>
@@ -4702,7 +5318,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D6" t="s">
         <v>81</v>
@@ -4716,7 +5332,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D7" t="s">
         <v>239</v>
@@ -4730,7 +5346,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D8" t="s">
         <v>211</v>
@@ -4744,7 +5360,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D9" t="s">
         <v>69</v>
@@ -4758,7 +5374,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D10" t="s">
         <v>58</v>
@@ -4814,7 +5430,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D14" t="s">
         <v>105</v>
@@ -4828,7 +5444,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D15" t="s">
         <v>134</v>
@@ -4848,7 +5464,7 @@
         <v>235</v>
       </c>
       <c r="E16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G16" t="s">
         <v>91</v>
@@ -4860,7 +5476,7 @@
         <v>198</v>
       </c>
       <c r="J16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4885,7 +5501,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D18" t="s">
         <v>99</v>
@@ -5063,7 +5679,7 @@
         <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J5" t="s">
         <v>146</v>
@@ -5083,7 +5699,7 @@
         <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J6" t="s">
         <v>142</v>
@@ -5103,7 +5719,7 @@
         <v>239</v>
       </c>
       <c r="E7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J7" t="s">
         <v>84</v>
@@ -5117,7 +5733,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D8" t="s">
         <v>211</v>
@@ -5291,7 +5907,7 @@
         <v>233</v>
       </c>
       <c r="E20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G20" t="s">
         <v>91</v>
@@ -5303,7 +5919,7 @@
         <v>198</v>
       </c>
       <c r="J20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5399,7 +6015,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -5413,7 +6029,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -5559,10 +6175,10 @@
         <v>27</v>
       </c>
       <c r="E13" t="s">
+        <v>312</v>
+      </c>
+      <c r="J13" t="s">
         <v>313</v>
-      </c>
-      <c r="J13" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5621,10 +6237,10 @@
         <v>35</v>
       </c>
       <c r="E17" t="s">
+        <v>314</v>
+      </c>
+      <c r="J17" t="s">
         <v>315</v>
-      </c>
-      <c r="J17" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -5683,10 +6299,10 @@
         <v>40</v>
       </c>
       <c r="E21" t="s">
+        <v>316</v>
+      </c>
+      <c r="J21" t="s">
         <v>317</v>
-      </c>
-      <c r="J21" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -5703,7 +6319,7 @@
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" t="s">
         <v>91</v>
@@ -5715,7 +6331,7 @@
         <v>198</v>
       </c>
       <c r="J22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -5760,10 +6376,10 @@
         <v>46</v>
       </c>
       <c r="E25" t="s">
+        <v>318</v>
+      </c>
+      <c r="J25" t="s">
         <v>319</v>
-      </c>
-      <c r="J25" t="s">
-        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -5824,7 +6440,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D2" t="s">
         <v>115</v>
@@ -5838,7 +6454,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D3" t="s">
         <v>86</v>
@@ -5987,7 +6603,7 @@
         <v>176</v>
       </c>
       <c r="J13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6049,7 +6665,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -6111,7 +6727,7 @@
         <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -6128,7 +6744,7 @@
         <v>68</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" t="s">
         <v>91</v>
@@ -6140,7 +6756,7 @@
         <v>198</v>
       </c>
       <c r="J22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -6188,7 +6804,7 @@
         <v>133</v>
       </c>
       <c r="J25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -6256,7 +6872,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -6270,7 +6886,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -6419,7 +7035,7 @@
         <v>176</v>
       </c>
       <c r="J13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -6481,7 +7097,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -6543,7 +7159,7 @@
         <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -6560,7 +7176,7 @@
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G22" t="s">
         <v>91</v>
@@ -6572,7 +7188,7 @@
         <v>198</v>
       </c>
       <c r="J22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -6620,7 +7236,7 @@
         <v>133</v>
       </c>
       <c r="J25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -6651,7 +7267,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B1" t="s">
         <v>166</v>
@@ -6743,7 +7359,7 @@
         <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -6916,7 +7532,7 @@
         <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J15" t="s">
         <v>178</v>
@@ -6950,7 +7566,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
@@ -6967,7 +7583,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D18" t="s">
         <v>36</v>
@@ -6984,7 +7600,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D19" t="s">
         <v>37</v>
@@ -7001,7 +7617,7 @@
         <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D20" t="s">
         <v>38</v>
@@ -7035,7 +7651,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D22" t="s">
         <v>42</v>
@@ -7052,7 +7668,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D23" t="s">
         <v>43</v>
@@ -7075,7 +7691,7 @@
         <v>44</v>
       </c>
       <c r="J24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -7099,25 +7715,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E99131-E2A9-44CA-9411-B82003F38B39}">
-  <dimension ref="A1:J33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D258555-A69A-4568-84CE-74B7B3743BDB}">
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -7163,7 +7771,7 @@
         <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -7174,10 +7782,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -7188,33 +7796,24 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" t="s">
-        <v>321</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>340</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" t="s">
-        <v>176</v>
-      </c>
-      <c r="J5" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -7222,19 +7821,13 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>341</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>189</v>
-      </c>
-      <c r="J6" t="s">
-        <v>192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -7242,56 +7835,41 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>267</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s">
-        <v>191</v>
-      </c>
-      <c r="J7" t="s">
-        <v>193</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>286</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" t="s">
-        <v>190</v>
-      </c>
-      <c r="J8" t="s">
-        <v>194</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>288</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -7299,395 +7877,247 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>274</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>71</v>
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>335</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>272</v>
       </c>
       <c r="D20" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>271</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" t="s">
-        <v>270</v>
-      </c>
-      <c r="G22" t="s">
-        <v>91</v>
-      </c>
-      <c r="H22" t="s">
-        <v>197</v>
-      </c>
-      <c r="I22" t="s">
-        <v>198</v>
-      </c>
-      <c r="J22" t="s">
-        <v>271</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>306</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>336</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>337</v>
+      </c>
+      <c r="J24" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>307</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>7</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" t="s">
-        <v>294</v>
-      </c>
-      <c r="J26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>7</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" t="s">
-        <v>293</v>
-      </c>
-      <c r="J27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>7</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>7</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>8</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" t="s">
-        <v>107</v>
-      </c>
-      <c r="E30" t="s">
-        <v>279</v>
-      </c>
-      <c r="J30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>8</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" t="s">
-        <v>297</v>
-      </c>
-      <c r="J31" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>8</v>
-      </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" t="s">
-        <v>296</v>
-      </c>
-      <c r="J32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>8</v>
-      </c>
-      <c r="B33">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" t="s">
-        <v>115</v>
-      </c>
-      <c r="E33" t="s">
-        <v>295</v>
-      </c>
-      <c r="J33" t="s">
-        <v>116</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>